<commit_message>
Adding 10 Manhattan plots lecture and recitation
</commit_message>
<xml_diff>
--- a/1_01_principles/files/schedule_modules.xlsx
+++ b/1_01_principles/files/schedule_modules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/dataviz-site/1_01_principles/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/dataviz-site/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="14_{322453E6-7958-7F45-A2A8-EC9083DB3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7602E64-0C92-C443-8878-B98EE972C50B}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="14_{322453E6-7958-7F45-A2A8-EC9083DB3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41530C99-CD23-AA48-8F4C-1A20EC680845}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
+    <workbookView xWindow="14120" yWindow="3580" windowWidth="28800" windowHeight="16360" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="24">
   <si>
     <t>Principles of data visualization</t>
   </si>
@@ -59,15 +59,9 @@
     <t>Principal components analysis</t>
   </si>
   <si>
-    <t>Manhattan plots</t>
-  </si>
-  <si>
     <t>Interactive plots</t>
   </si>
   <si>
-    <t>Making lots of plots at once</t>
-  </si>
-  <si>
     <t>Capstone assignment open session</t>
   </si>
   <si>
@@ -101,7 +95,19 @@
     <t>Themes, labels, facets (ggplot 102)</t>
   </si>
   <si>
-    <t>Open for input</t>
+    <t>Open session, capstone prep</t>
+  </si>
+  <si>
+    <t>Manhattan plots and making lots of plots at once</t>
+  </si>
+  <si>
+    <t>ggplot extension packages and complexheatmap</t>
+  </si>
+  <si>
+    <t>No class, Thanksgiving</t>
+  </si>
+  <si>
+    <t>Relaxing and eating</t>
   </si>
 </sst>
 </file>
@@ -454,26 +460,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F342C0D-B564-AC4C-B9F2-1430BA1BF96D}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -481,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -492,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -503,7 +509,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -514,10 +520,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -525,10 +531,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -536,7 +542,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -547,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -558,10 +564,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -569,10 +575,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,10 +586,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -591,10 +597,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -602,10 +608,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -613,10 +619,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,10 +630,32 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -639,30 +667,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AC0B77-377C-2E43-B142-D9BC271E0496}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -673,7 +699,7 @@
         <v>44796</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -687,7 +713,7 @@
         <v>44803</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -701,7 +727,7 @@
         <v>44810</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -715,10 +741,10 @@
         <v>44817</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -729,10 +755,10 @@
         <v>44825</v>
       </c>
       <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -743,7 +769,7 @@
         <v>44832</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -757,7 +783,7 @@
         <v>44838</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -771,10 +797,10 @@
         <v>44845</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -785,10 +811,10 @@
         <v>44852</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -799,10 +825,10 @@
         <v>44859</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -813,10 +839,10 @@
         <v>44866</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -827,10 +853,10 @@
         <v>44873</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -841,7 +867,7 @@
         <v>44880</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -855,10 +881,10 @@
         <v>44887</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -869,10 +895,10 @@
         <v>44894</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -880,13 +906,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>44901</v>
+        <v>44900</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>